<commit_message>
Change background style and MS font size
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Typography" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="112">
   <si>
     <t xml:space="preserve">TouchGFX - Typography Sheet</t>
   </si>
@@ -354,6 +354,12 @@
   </si>
   <si>
     <t xml:space="preserve">msw_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TextId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text</t>
   </si>
 </sst>
 </file>
@@ -754,25 +760,25 @@
   </sheetPr>
   <dimension ref="B1:O15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="0.319838056680162"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.1376518218623"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="1" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="54.0931174089069"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="54.5222672064777"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="98.336032388664"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="99.1902834008097"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1136,7 +1142,7 @@
         <v>33</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>4</v>
@@ -1191,19 +1197,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:K30"/>
+  <dimension ref="B1:K31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="0.319838056680162"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.5627530364373"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="40.919028340081"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="58.4858299595142"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.8866396761134"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="41.2388663967611"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="58.914979757085"/>
     <col collapsed="false" hidden="false" max="10" min="8" style="1" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
   </cols>
@@ -1655,6 +1661,20 @@
       </c>
       <c r="F30" s="1" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix status update. Remove unused screens and custom transition
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -2,26 +2,26 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <workbookPr autoCompressPictures="1"/>
+  <workbookProtection lockStructure="0" lockWindows="0" lockRevision="0"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView windowWidth="16384" windowHeight="8192" tabRatio="992"/>
   </bookViews>
   <sheets>
-    <sheet name="Typography" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Translation" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Typography" sheetId="1" r:id="rId2"/>
+    <sheet name="Translation" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcMode="auto" fullCalcOnLoad="0" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001" fullPrecision="0" calcCompleted="0" calcOnSave="0" concurrentCalc="0" forceFullCalc="0"/>
   <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    <ext uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr xmlns:loext="http://schemas.libreoffice.org/" stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5893" uniqueCount="112">
   <si>
     <t xml:space="preserve">TouchGFX - Typography Sheet</t>
   </si>
@@ -755,40 +755,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+  <sheetPr>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="B1:O15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView showGridLines="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="0.319838056680162"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="54.5222672064777"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="99.1902834008097"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.57085020242915"/>
+    <col min="1" max="1" width="0.319838056680162" style="0"/>
+    <col min="2" max="2" width="29.1376518218623" style="1"/>
+    <col min="3" max="3" width="32.1376518218623" style="1"/>
+    <col min="4" max="5" width="7.49797570850202" style="1"/>
+    <col min="6" max="6" width="19.4939271255061" style="0"/>
+    <col min="7" max="7" width="54.5222672064777" style="0"/>
+    <col min="8" max="9" width="23.4574898785425" style="0"/>
+    <col min="10" max="10" width="4.39271255060729" style="0"/>
+    <col min="11" max="11" width="22.6032388663968" style="0"/>
+    <col min="12" max="12" width="99.1902834008097" style="0"/>
+    <col min="13" max="13" width="13.3886639676113" style="0"/>
+    <col min="14" max="14" width="11.0323886639676" style="0"/>
+    <col min="15" max="15" width="21.3157894736842" style="0"/>
+    <col min="16" max="1025" width="8.57085020242915" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="129" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0"/>
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
-      <c r="E1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" ht="129" hidden="1" customHeight="1">
+      <c r="B1"/>
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1"/>
+    </row>
+    <row r="2" ht="39.95" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -800,7 +800,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" ht="15.75">
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
@@ -826,28 +826,29 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="s">
+    <row r="4" ht="15">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4">
         <v>16</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4">
         <v>4</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" t="s">
         <v>13</v>
       </c>
+      <c r="I4"/>
       <c r="K4" s="7" t="s">
         <v>14</v>
       </c>
@@ -864,94 +865,99 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1" t="s">
+    <row r="5" ht="15">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5">
         <v>20</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" t="s">
         <v>13</v>
       </c>
+      <c r="I5"/>
       <c r="K5" s="10" t="s">
         <v>3</v>
       </c>
       <c r="L5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M5" s="12" t="n">
+      <c r="M5" s="12">
         <v>20</v>
       </c>
-      <c r="N5" s="12" t="n">
+      <c r="N5" s="12">
         <v>36</v>
       </c>
       <c r="O5" s="13"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1" t="s">
+    <row r="6" ht="13.8">
+      <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6">
         <v>24</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6">
         <v>4</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="F6"/>
+      <c r="G6" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="H6" t="s">
         <v>13</v>
       </c>
+      <c r="I6"/>
       <c r="K6" s="10" t="s">
         <v>4</v>
       </c>
       <c r="L6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="M6" s="12" t="n">
+      <c r="M6" s="12">
         <v>4</v>
       </c>
-      <c r="N6" s="12" t="n">
+      <c r="N6" s="12">
         <v>8</v>
       </c>
       <c r="O6" s="13"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="s">
+    <row r="7" ht="13.8">
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7">
         <v>55</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7">
         <v>4</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="F7"/>
+      <c r="G7" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" t="s">
         <v>13</v>
       </c>
+      <c r="I7"/>
       <c r="K7" s="10" t="s">
         <v>5</v>
       </c>
@@ -968,25 +974,27 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
+    <row r="8" ht="13.8">
+      <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8">
         <v>30</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8">
         <v>4</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="F8"/>
+      <c r="G8" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" t="s">
         <v>13</v>
       </c>
+      <c r="I8"/>
       <c r="K8" s="10" t="s">
         <v>6</v>
       </c>
@@ -1001,25 +1009,27 @@
       </c>
       <c r="O8" s="13"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1" t="s">
+    <row r="9" ht="13.8">
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9">
         <v>28</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9">
         <v>4</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="F9"/>
+      <c r="G9" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="H9" t="s">
         <v>13</v>
       </c>
+      <c r="I9"/>
       <c r="K9" s="14" t="s">
         <v>7</v>
       </c>
@@ -1036,25 +1046,27 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1" t="s">
+    <row r="10" ht="13.8">
+      <c r="B10" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10">
         <v>28</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10">
         <v>4</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="F10"/>
+      <c r="G10" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="H10" t="s">
         <v>13</v>
       </c>
+      <c r="I10"/>
       <c r="K10" s="14" t="s">
         <v>8</v>
       </c>
@@ -1069,119 +1081,129 @@
       </c>
       <c r="O10" s="17"/>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1" t="s">
+    <row r="11" ht="13.8">
+      <c r="B11" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11">
         <v>28</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11">
         <v>4</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="F11"/>
+      <c r="G11" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="H11" t="s">
         <v>13</v>
       </c>
+      <c r="I11"/>
       <c r="K11" s="19"/>
       <c r="L11" s="20"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
+    <row r="12" ht="13.8">
+      <c r="B12" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12">
         <v>20</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12">
         <v>4</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="F12"/>
+      <c r="G12" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="0" t="s">
+      <c r="H12" t="s">
         <v>13</v>
       </c>
+      <c r="I12"/>
       <c r="L12" s="20" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1" t="s">
+    <row r="13" ht="13.8">
+      <c r="B13" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13">
         <v>20</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13">
         <v>4</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="F13"/>
+      <c r="G13" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="0" t="s">
+      <c r="H13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1" t="s">
+      <c r="I13"/>
+    </row>
+    <row r="14" ht="13.8">
+      <c r="B14" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14">
         <v>18</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14">
         <v>4</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="F14"/>
+      <c r="G14" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="0" t="s">
+      <c r="H14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1" t="s">
+      <c r="I14"/>
+    </row>
+    <row r="15" ht="13.8">
+      <c r="B15" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15">
         <v>16</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15">
         <v>4</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="F15"/>
+      <c r="G15" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="H15" t="s">
         <v>13</v>
       </c>
+      <c r="I15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:H2"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" orientation="portrait" usePrinterDefaults="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter>
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
@@ -1194,38 +1216,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+  <sheetPr>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="B1:K31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+    <sheetView showGridLines="0" showOutlineSymbols="1" defaultGridColor="1" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="0.319838056680162"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.8866396761134"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="41.2388663967611"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="58.914979757085"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="1" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
+    <col min="1" max="1" width="0.319838056680162" style="0"/>
+    <col min="2" max="2" width="35.8866396761134" style="1"/>
+    <col min="3" max="4" width="29.1376518218623" style="1"/>
+    <col min="5" max="6" width="41.2388663967611" style="1"/>
+    <col min="7" max="7" width="58.914979757085" style="1"/>
+    <col min="8" max="10" width="8.67611336032389" style="1"/>
+    <col min="11" max="1025" width="8.57085020242915" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="129" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0"/>
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
-      <c r="H1" s="0"/>
-      <c r="I1" s="0"/>
-      <c r="J1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" ht="129" hidden="1" customHeight="1">
+      <c r="B1"/>
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+    </row>
+    <row r="2" ht="39.95" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>48</v>
       </c>
@@ -1237,11 +1259,11 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="0" t="s">
+      <c r="K2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" ht="13.8">
       <c r="B3" s="1" t="s">
         <v>50</v>
       </c>
@@ -1270,410 +1292,433 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="s">
+    <row r="4" ht="13.8">
+      <c r="B4" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1" t="s">
+    <row r="5" ht="13.8">
+      <c r="B5" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1" t="s">
+    <row r="6" ht="13.8">
+      <c r="B6" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="s">
+    <row r="7" ht="13.8">
+      <c r="B7" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>69</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
+    <row r="8" ht="41.75">
+      <c r="B8" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>64</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1" t="s">
+    <row r="9" ht="13.8">
+      <c r="B9" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>69</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="E9"/>
+      <c r="F9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1" t="s">
+    <row r="10" ht="13.8">
+      <c r="B10" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="E10"/>
+      <c r="F10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1" t="s">
+    <row r="11" ht="13.8">
+      <c r="B11" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="E11"/>
+      <c r="F11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
+    <row r="12" ht="13.8">
+      <c r="B12" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>69</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="E12"/>
+      <c r="F12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1" t="s">
+    <row r="13" ht="13.8">
+      <c r="B13" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="E13"/>
+      <c r="F13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1" t="s">
+    <row r="14" ht="13.8">
+      <c r="B14" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="E14"/>
+      <c r="F14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1" t="s">
+    <row r="15" ht="13.8">
+      <c r="B15" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="E15"/>
+      <c r="F15" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1" t="s">
+    <row r="16" ht="13.8">
+      <c r="B16" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="E16"/>
+      <c r="F16" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="1" t="s">
+    <row r="17" ht="13.8">
+      <c r="B17" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="E17"/>
+      <c r="F17" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="1" t="s">
+    <row r="18" ht="13.8">
+      <c r="B18" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="E18"/>
+      <c r="F18" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="1" t="s">
+    <row r="19" ht="13.8">
+      <c r="B19" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="E19"/>
+      <c r="F19" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="1" t="s">
+    <row r="20" ht="13.8">
+      <c r="B20" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="E20"/>
+      <c r="F20" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="1" t="s">
+    <row r="21" ht="13.8">
+      <c r="B21" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="E21"/>
+      <c r="F21" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="1" t="s">
+    <row r="22" ht="13.8">
+      <c r="B22" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>69</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="E22"/>
+      <c r="F22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="1" t="s">
+    <row r="23" ht="13.8">
+      <c r="B23" t="s">
         <v>99</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>63</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="E23"/>
+      <c r="F23" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="1" t="s">
+    <row r="24" ht="13.8">
+      <c r="B24" t="s">
         <v>101</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="E24"/>
+      <c r="F24" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="1" t="s">
+    <row r="25" ht="13.8">
+      <c r="B25" t="s">
         <v>103</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="E25"/>
+      <c r="F25" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="1" t="s">
+    <row r="26" ht="13.8">
+      <c r="B26" t="s">
         <v>105</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>63</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="E26"/>
+      <c r="F26" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="1" t="s">
+    <row r="27" ht="13.8">
+      <c r="B27" t="s">
         <v>106</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>69</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="E27"/>
+      <c r="F27" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="1" t="s">
+    <row r="28" ht="13.8">
+      <c r="B28" t="s">
         <v>107</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="E28"/>
+      <c r="F28" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="1" t="s">
+    <row r="29" ht="13.8">
+      <c r="B29" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>63</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="E29"/>
+      <c r="F29" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="1" t="s">
+    <row r="30" ht="13.8">
+      <c r="B30" t="s">
         <v>109</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" t="s">
         <v>69</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="E30"/>
+      <c r="F30" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="1" t="s">
+    <row r="31" ht="13.8">
+      <c r="B31" t="s">
         <v>110</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>69</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="E31"/>
+      <c r="F31" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1681,10 +1726,10 @@
   <mergeCells count="1">
     <mergeCell ref="B2:J2"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" orientation="portrait" usePrinterDefaults="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter>
     <oddHeader/>
     <oddFooter/>
   </headerFooter>

</xml_diff>